<commit_message>
ricalcolo qta moq/bancale, sembra ok, chiedere per ricalolo finale al bancale CALCOLA-QTA-ORD e per la data che è sempre uguale, manca il controllo in ananagrafica articolo
</commit_message>
<xml_diff>
--- a/ricalcolo scorta.xlsx
+++ b/ricalcolo scorta.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>QTA MESE 1</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>TOT-QTA-MESE6</t>
+  </si>
+  <si>
+    <t>ECCESSO</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +454,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -465,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -473,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -481,7 +484,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -489,7 +492,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -497,7 +500,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -505,7 +508,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>250</v>
+        <v>720</v>
       </c>
       <c r="C8" t="str">
         <f>IF(B8&gt;=B9,"X","")</f>
@@ -518,7 +521,7 @@
       </c>
       <c r="B9">
         <f>B1+B2+B3+B4+B5+B6</f>
-        <v>1350</v>
+        <v>1050</v>
       </c>
       <c r="C9" t="str">
         <f>IF(B9&gt;=B8,"X","")</f>
@@ -531,7 +534,7 @@
       </c>
       <c r="B11">
         <f>IF(B9&gt;B8,B9,B8)</f>
-        <v>1350</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -540,7 +543,7 @@
       </c>
       <c r="B13">
         <f>IF(B11&gt;F1,CEILING(B11/F1,1),1)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -549,7 +552,7 @@
       </c>
       <c r="B15">
         <f>F1*B13</f>
-        <v>1500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -558,7 +561,7 @@
       </c>
       <c r="B16">
         <f>B1+B2</f>
-        <v>250</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -567,7 +570,7 @@
       </c>
       <c r="B17">
         <f>B1+B2+B3</f>
-        <v>450</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,7 +579,7 @@
       </c>
       <c r="B18">
         <f>B1+B2+B3+B4</f>
-        <v>700</v>
+        <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -585,7 +588,7 @@
       </c>
       <c r="B19">
         <f>B1+B2+B3+B4+B5</f>
-        <v>1000</v>
+        <v>750</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -594,7 +597,7 @@
       </c>
       <c r="B20">
         <f>B1+B2+B3+B4+B5+B6</f>
-        <v>1350</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -616,29 +619,29 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f>B1</f>
-        <v>100</v>
+        <f t="shared" ref="B23:B28" si="0">B1</f>
+        <v>50</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
         <f>B23</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E23">
-        <f>IF(D23&gt;$F$1,ARROTOND.ECCESSO(D23/$F$1,1),1)</f>
+        <f>IF(D23&gt;$F$1,CEILING(D23/$F$1,1),1)</f>
         <v>1</v>
       </c>
       <c r="F23" s="2">
-        <f>E23*$F$1</f>
+        <f t="shared" ref="F23:F28" si="1">E23*$F$1</f>
         <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24">
-        <f>B2</f>
-        <v>150</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="C24">
         <f>F23</f>
@@ -646,21 +649,21 @@
       </c>
       <c r="D24">
         <f>B16-C24</f>
-        <v>-50</v>
+        <v>-150</v>
       </c>
       <c r="E24">
         <f>IF(D24&gt;0,IF(D24&gt;$F$1,CEILING(D24/$F$1,1),1),0)</f>
         <v>0</v>
       </c>
       <c r="F24" s="2">
-        <f>E24*$F$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25">
-        <f>B3</f>
-        <v>200</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
       <c r="C25">
         <f>F23+F24</f>
@@ -668,69 +671,69 @@
       </c>
       <c r="D25">
         <f>B17-C25</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <f>IF(D25&gt;0,IF(D25&gt;$F$1,CEILING(D25/$F$1,1),1),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="2">
-        <f>E25*$F$1</f>
-        <v>300</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26">
-        <f>B4</f>
-        <v>250</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="C26">
         <f>F23+F24+F25</f>
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="D26">
         <f>B18-C26</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E26">
         <f>IF(D26&gt;0,IF(D26&gt;$F$1,CEILING(D26/$F$1,1),1),0)</f>
         <v>1</v>
       </c>
       <c r="F26" s="2">
-        <f>E26*$F$1</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27">
-        <f>B5</f>
-        <v>300</v>
+        <f t="shared" si="0"/>
+        <v>250</v>
       </c>
       <c r="C27">
         <f>F23+F24+F25+F26</f>
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="D27">
         <f>B19-C27</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E27">
         <f>IF(D27&gt;0,IF(D27&gt;$F$1,CEILING(D27/$F$1,1),1),0)</f>
         <v>1</v>
       </c>
       <c r="F27" s="2">
-        <f>E27*$F$1</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28">
-        <f>B6</f>
-        <v>350</v>
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
       <c r="C28">
         <f>F23+F24+F25+F26+F27</f>
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="D28">
         <f>B15-C28</f>
@@ -741,14 +744,14 @@
         <v>1</v>
       </c>
       <c r="F28" s="2">
-        <f>E28*$F$1</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F30" s="2">
         <f>SUM(F23:F28)</f>
-        <v>1500</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -758,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,8 +774,8 @@
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -780,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -794,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -808,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,7 +819,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -824,7 +827,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -832,7 +835,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,7 +843,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="C8" t="str">
         <f>IF(B8&gt;=B9,"X","")</f>
@@ -853,7 +856,7 @@
       </c>
       <c r="B9">
         <f>B1+B2+B3+B4+B5+B6</f>
-        <v>1350</v>
+        <v>1050</v>
       </c>
       <c r="C9" t="str">
         <f>IF(B9&gt;=B8,"X","")</f>
@@ -866,7 +869,7 @@
       </c>
       <c r="B11">
         <f>IF(B9&gt;B8,B9,B8)</f>
-        <v>1350</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,7 +878,7 @@
       </c>
       <c r="B13">
         <f>IF(B11&gt;F1,CEILING(B11/F1,1),1)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,7 +887,7 @@
       </c>
       <c r="B15">
         <f>F1*B13</f>
-        <v>1500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,46 +896,46 @@
       </c>
       <c r="B16">
         <f>B1+B2</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17">
         <f>B1+B2+B3</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18">
         <f>B1+B2+B3+B4</f>
-        <v>700</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19">
         <f>B1+B2+B3+B4+B5</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20">
         <f>B1+B2+B3+B4+B5+B6</f>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>9</v>
       </c>
@@ -943,259 +946,228 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
       <c r="H22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J22" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f>B1</f>
-        <v>100</v>
+        <f t="shared" ref="B23:B28" si="0">B1</f>
+        <v>50</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
         <f>B23</f>
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <f>CEILING(D23/$B$8,1)</f>
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ref="F23:F28" si="1">E23*$B$8</f>
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G28" si="2">FLOOR(F23/$F$1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>F23-G23*$F$1</f>
+        <v>50</v>
+      </c>
+      <c r="I23" s="2">
+        <f>IF(H23&gt;$F$1*$F$2,(G23+1)*$F$1,F23)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="E23">
-        <f>IF(D23&gt;$F$1,CEILING(D23/$F$1,1),1)</f>
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <f>E23*$F$1</f>
-        <v>300</v>
-      </c>
-      <c r="H23">
-        <f>CEILING(F23/$B$8,1)</f>
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <f>H23*$B$8</f>
-        <v>500</v>
-      </c>
-      <c r="J23">
-        <f>FLOOR(I23/$F$1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="K23" s="2">
-        <f>IF(I23&gt;($F$1*J23+($F$1*$F$2)),(J23+1)*$F$1,J23*$F$1)</f>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <f>B2</f>
-        <v>150</v>
-      </c>
       <c r="C24">
-        <f>K23</f>
-        <v>600</v>
+        <f>I23</f>
+        <v>50</v>
       </c>
       <c r="D24">
         <f>B16-C24</f>
-        <v>-350</v>
+        <v>100</v>
       </c>
       <c r="E24">
-        <f>IF(D24&gt;0,IF(D24&gt;$F$1,CEILING(D24/$F$1,1),1),0)</f>
-        <v>0</v>
+        <f>CEILING(D24/$B$8,1)</f>
+        <v>10</v>
       </c>
       <c r="F24">
-        <f>E24*$F$1</f>
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H24">
-        <f>CEILING(F24/$B$8,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <f>H24*$B$8</f>
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <f>FLOOR(I24/$F$1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="2">
-        <f>IF(I24&gt;($F$1*J24+($F$1*$F$2)),(J24+1)*$F$1,J24*$F$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <f>F24-G24*$F$1</f>
+        <v>100</v>
+      </c>
+      <c r="I24" s="2">
+        <f>IF(H24&gt;$F$1*$F$2,(G24+1)*$F$1,F24)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25">
-        <f>B3</f>
-        <v>200</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
       <c r="C25">
-        <f>K23+K24</f>
-        <v>600</v>
+        <f>I23+I24</f>
+        <v>150</v>
       </c>
       <c r="D25">
         <f>B17-C25</f>
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="E25">
-        <f>IF(D25&gt;0,IF(D25&gt;$F$1,CEILING(D25/$F$1,1),1),0)</f>
-        <v>0</v>
+        <f>CEILING(D25/$B$8,1)</f>
+        <v>15</v>
       </c>
       <c r="F25">
-        <f>E25*$F$1</f>
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H25">
-        <f>CEILING(F25/$B$8,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <f>H25*$B$8</f>
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <f>FLOOR(I25/$F$1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="2">
-        <f>IF(I25&gt;($F$1*J25+($F$1*$F$2)),(J25+1)*$F$1,J25*$F$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <f>F25-G25*$F$1</f>
+        <v>150</v>
+      </c>
+      <c r="I25" s="2">
+        <f>IF(H25&gt;$F$1*$F$2,(G25+1)*$F$1,F25)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26">
-        <f>B4</f>
-        <v>250</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="C26">
-        <f>K23+K24+K25</f>
-        <v>600</v>
+        <f>I23+I24+I25</f>
+        <v>300</v>
       </c>
       <c r="D26">
         <f>B18-C26</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E26">
-        <f>IF(D26&gt;0,IF(D26&gt;$F$1,CEILING(D26/$F$1,1),1),0)</f>
-        <v>1</v>
+        <f>CEILING(D26/$B$8,1)</f>
+        <v>20</v>
       </c>
       <c r="F26">
-        <f>E26*$F$1</f>
-        <v>300</v>
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="H26">
-        <f>CEILING(F26/$B$8,1)</f>
-        <v>2</v>
-      </c>
-      <c r="I26">
-        <f>H26*$B$8</f>
-        <v>500</v>
-      </c>
-      <c r="J26">
-        <f>FLOOR(I26/$F$1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="K26" s="2">
-        <f>IF(I26&gt;($F$1*J26+($F$1*$F$2)),(J26+1)*$F$1,J26*$F$1)</f>
+        <f>F26-G26*$F$1</f>
+        <v>200</v>
+      </c>
+      <c r="I26" s="2">
+        <f>IF(H26&gt;$F$1*$F$2,(G26+1)*$F$1,F26)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="C27">
+        <f>I23+I24+I25+I26</f>
         <v>600</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <f>B5</f>
-        <v>300</v>
-      </c>
-      <c r="C27">
-        <f>K23+K24+K25+K26</f>
-        <v>1200</v>
       </c>
       <c r="D27">
         <f>B19-C27</f>
-        <v>-200</v>
+        <v>150</v>
       </c>
       <c r="E27">
-        <f>IF(D27&gt;0,IF(D27&gt;$F$1,CEILING(D27/$F$1,1),1),0)</f>
-        <v>0</v>
+        <f>CEILING(D27/$B$8,1)</f>
+        <v>15</v>
       </c>
       <c r="F27">
-        <f>E27*$F$1</f>
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H27">
-        <f>CEILING(F27/$B$8,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <f>H27*$B$8</f>
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <f>FLOOR(I27/$F$1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="2">
-        <f>IF(I27&gt;($F$1*J27+($F$1*$F$2)),(J27+1)*$F$1,J27*$F$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <f>F27-G27*$F$1</f>
+        <v>150</v>
+      </c>
+      <c r="I27" s="2">
+        <f>IF(H27&gt;$F$1*$F$2,(G27+1)*$F$1,F27)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28">
-        <f>B6</f>
-        <v>350</v>
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
       <c r="C28">
-        <f>K23+K24+K25+K26+K27</f>
-        <v>1200</v>
+        <f>I23+I24+I25+I26+I27</f>
+        <v>750</v>
       </c>
       <c r="D28">
         <f>B15-C28</f>
-        <v>300</v>
+        <v>450</v>
       </c>
       <c r="E28">
-        <f>IF(D28&gt;0,IF(D28&gt;$F$1,CEILING(D28/$F$1,1),1),0)</f>
+        <f>CEILING(D28/$B$8,1)</f>
+        <v>45</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="F28">
-        <f>E28*$F$1</f>
-        <v>300</v>
-      </c>
       <c r="H28">
-        <f>CEILING(F28/$B$8,1)</f>
-        <v>2</v>
-      </c>
-      <c r="I28">
-        <f>H28*$B$8</f>
-        <v>500</v>
-      </c>
-      <c r="J28">
-        <f>FLOOR(I28/$F$1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="K28" s="2">
-        <f>IF(I28&gt;($F$1*J28+($F$1*$F$2)),(J28+1)*$F$1,J28*$F$1)</f>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F30">
-        <f>SUM(F23:F28)</f>
-        <v>900</v>
-      </c>
-      <c r="K30">
-        <f>SUM(K23:K28)</f>
-        <v>1800</v>
+        <f>F28-G28*$F$1</f>
+        <v>150</v>
+      </c>
+      <c r="I28" s="2">
+        <f>IF(H28&gt;$F$1*$F$2,(G28+1)*$F$1,F28)</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f>SUM(I23:I28)</f>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunto ricalcolo moq su ordini f non auto, sistemare il log
</commit_message>
<xml_diff>
--- a/ricalcolo scorta.xlsx
+++ b/ricalcolo scorta.xlsx
@@ -761,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +843,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" t="str">
         <f>IF(B8&gt;=B9,"X","")</f>
@@ -974,24 +974,24 @@
         <v>50</v>
       </c>
       <c r="E23">
-        <f>CEILING(D23/$B$8,1)</f>
+        <f t="shared" ref="E23:E28" si="1">CEILING(D23/$B$8,1)</f>
         <v>5</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:F28" si="1">E23*$B$8</f>
-        <v>50</v>
+        <f t="shared" ref="F23:F28" si="2">E23*$B$8</f>
+        <v>60</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G28" si="2">FLOOR(F23/$F$1,1)</f>
+        <f t="shared" ref="G23:G28" si="3">FLOOR(F23/$F$1,1)</f>
         <v>0</v>
       </c>
       <c r="H23">
-        <f>F23-G23*$F$1</f>
-        <v>50</v>
+        <f t="shared" ref="H23:H28" si="4">F23-G23*$F$1</f>
+        <v>60</v>
       </c>
       <c r="I23" s="2">
-        <f>IF(H23&gt;$F$1*$F$2,(G23+1)*$F$1,F23)</f>
-        <v>50</v>
+        <f t="shared" ref="I23:I28" si="5">IF(H23&gt;$F$1*$F$2,(G23+1)*$F$1,F23)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1001,31 +1001,31 @@
       </c>
       <c r="C24">
         <f>I23</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D24">
         <f>B16-C24</f>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E24">
-        <f>CEILING(D24/$B$8,1)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>96</v>
       </c>
       <c r="G24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H24">
-        <f>F24-G24*$F$1</f>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>96</v>
       </c>
       <c r="I24" s="2">
-        <f>IF(H24&gt;$F$1*$F$2,(G24+1)*$F$1,F24)</f>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1035,31 +1035,31 @@
       </c>
       <c r="C25">
         <f>I23+I24</f>
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D25">
         <f>B17-C25</f>
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E25">
-        <f>CEILING(D25/$B$8,1)</f>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" si="2"/>
+        <v>144</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H25">
-        <f>F25-G25*$F$1</f>
-        <v>150</v>
+        <f t="shared" si="4"/>
+        <v>144</v>
       </c>
       <c r="I25" s="2">
-        <f>IF(H25&gt;$F$1*$F$2,(G25+1)*$F$1,F25)</f>
-        <v>150</v>
+        <f t="shared" si="5"/>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1076,23 +1076,23 @@
         <v>200</v>
       </c>
       <c r="E26">
-        <f>CEILING(D26/$B$8,1)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <f t="shared" si="2"/>
+        <v>204</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H26">
-        <f>F26-G26*$F$1</f>
-        <v>200</v>
+        <f t="shared" si="4"/>
+        <v>204</v>
       </c>
       <c r="I26" s="2">
-        <f>IF(H26&gt;$F$1*$F$2,(G26+1)*$F$1,F26)</f>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
     </row>
@@ -1110,24 +1110,24 @@
         <v>150</v>
       </c>
       <c r="E27">
-        <f>CEILING(D27/$B$8,1)</f>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" si="2"/>
+        <v>156</v>
       </c>
       <c r="G27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H27">
-        <f>F27-G27*$F$1</f>
-        <v>150</v>
+        <f t="shared" si="4"/>
+        <v>156</v>
       </c>
       <c r="I27" s="2">
-        <f>IF(H27&gt;$F$1*$F$2,(G27+1)*$F$1,F27)</f>
-        <v>150</v>
+        <f t="shared" si="5"/>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1137,37 +1137,43 @@
       </c>
       <c r="C28">
         <f>I23+I24+I25+I26+I27</f>
-        <v>750</v>
+        <v>900</v>
       </c>
       <c r="D28">
         <f>B15-C28</f>
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="E28">
-        <f>CEILING(D28/$B$8,1)</f>
-        <v>45</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
-        <v>450</v>
+        <f t="shared" si="2"/>
+        <v>300</v>
       </c>
       <c r="G28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H28">
-        <f>F28-G28*$F$1</f>
-        <v>150</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="I28" s="2">
-        <f>IF(H28&gt;$F$1*$F$2,(G28+1)*$F$1,F28)</f>
-        <v>450</v>
+        <f t="shared" si="5"/>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I29">
         <f>SUM(I23:I28)</f>
         <v>1200</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f>90/12</f>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>